<commit_message>
Split code into multiple files
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>59.79</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32.81</v>
+        <v>0.9399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -554,19 +554,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3960</v>
+        <v>1080</v>
       </c>
       <c r="D2" t="n">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
         <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>1190</v>
+        <v>810</v>
       </c>
       <c r="G2" t="n">
-        <v>286.5</v>
+        <v>122.38</v>
       </c>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3960</v>
+        <v>1080</v>
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3960</v>
+        <v>1080</v>
       </c>
       <c r="D4" t="n">
-        <v>290</v>
+        <v>66</v>
       </c>
       <c r="E4" t="n">
         <v>6</v>
       </c>
       <c r="F4" t="n">
-        <v>1094</v>
+        <v>810</v>
       </c>
       <c r="G4" t="n">
-        <v>61.18</v>
+        <v>35.02</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>290</v>
+        <v>66</v>
       </c>
       <c r="D5" t="n">
-        <v>290</v>
+        <v>66</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
@@ -655,7 +655,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
+          <t>Work with REO RPO to Correct (5.5.13.3)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -664,110 +664,86 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>272</v>
+        <v>17</v>
       </c>
       <c r="D6" t="n">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="F6" t="n">
-        <v>1184</v>
+        <v>166</v>
       </c>
       <c r="G6" t="n">
-        <v>84.26000000000001</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1490</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1167</v>
-      </c>
-      <c r="K6" t="n">
-        <v>41.39</v>
-      </c>
+        <v>128.67</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Create/Post Journal Entries (5.5.13.4)</t>
+          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Stop</t>
+          <t>Activity Step</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>133</v>
+        <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>127</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="F7" t="n">
-        <v>1190</v>
+        <v>168</v>
       </c>
       <c r="G7" t="n">
-        <v>109.38</v>
-      </c>
-      <c r="H7" t="n">
-        <v>77</v>
-      </c>
-      <c r="I7" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" t="n">
-        <v>5</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2.96</v>
-      </c>
+        <v>132.33</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Work with REO RPO to Correct (5.5.13.3)</t>
+          <t>Create/Post Journal Entries (5.5.13.4)</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Activity Step</t>
+          <t>Stop</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="F8" t="n">
-        <v>1180</v>
+        <v>174</v>
       </c>
       <c r="G8" t="n">
-        <v>481.95</v>
-      </c>
-      <c r="H8" t="n">
-        <v>3</v>
-      </c>
-      <c r="I8" t="n">
-        <v>3</v>
-      </c>
-      <c r="J8" t="n">
-        <v>3</v>
-      </c>
-      <c r="K8" t="n">
-        <v>3</v>
-      </c>
+        <v>137.67</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Need to fix code that writes to the simulation report.  Missing most information now.
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>11.5</v>
+        <v>99.77</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9399999999999999</v>
+        <v>39.55</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,197 +554,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1080</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" t="n">
-        <v>810</v>
-      </c>
-      <c r="G2" t="n">
-        <v>122.38</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Monthly</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Start</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1080</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Review AM using Asset Change Tracker (5.5.13.1)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1080</v>
-      </c>
-      <c r="D4" t="n">
-        <v>66</v>
-      </c>
-      <c r="E4" t="n">
-        <v>6</v>
-      </c>
-      <c r="F4" t="n">
-        <v>810</v>
-      </c>
-      <c r="G4" t="n">
-        <v>35.02</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Complete /Accurate?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Gateway</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>66</v>
-      </c>
-      <c r="D5" t="n">
-        <v>66</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Work with REO RPO to Correct (5.5.13.3)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>17</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>86</v>
-      </c>
-      <c r="F6" t="n">
-        <v>166</v>
-      </c>
-      <c r="G6" t="n">
-        <v>128.67</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>90</v>
-      </c>
-      <c r="F7" t="n">
-        <v>168</v>
-      </c>
-      <c r="G7" t="n">
-        <v>132.33</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Create/Post Journal Entries (5.5.13.4)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Stop</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>95</v>
-      </c>
-      <c r="F8" t="n">
-        <v>174</v>
-      </c>
-      <c r="G8" t="n">
-        <v>137.67</v>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed some of the missing information from the simulation rpt.  Simulation results still not similar to Bizagi simulation reults.
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>99.77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>39.55</v>
+        <v>45.35</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,27 +545,236 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5.5.13 Real Property-Monthly Reviews-org</t>
+          <t>Review AM using Asset Change Tracker (5.5.13.1)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Process</t>
+          <t>Activity Step</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+        <v>146</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" t="n">
+        <v>13</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Complete /Accurate?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Gateway</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>146</v>
+      </c>
+      <c r="D3" t="n">
+        <v>146</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Work with REO RPO to Correct (5.5.13.3)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Activity Step</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>60</v>
+      </c>
+      <c r="D4" t="n">
+        <v>60</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>165</v>
+      </c>
+      <c r="G4" t="n">
+        <v>117.12</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Activity Step</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>147</v>
+      </c>
+      <c r="D5" t="n">
+        <v>147</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1698</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>165</v>
+      </c>
+      <c r="K5" t="n">
+        <v>22.64</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Create/Post Journal Entries (5.5.13.4)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Stop</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>144</v>
+      </c>
+      <c r="D6" t="n">
+        <v>144</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Stop</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>144</v>
+      </c>
+      <c r="D7" t="n">
+        <v>144</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Wait time still not accurate.  fixed path and now correctly setting Start and Stop activities in path.
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>45.35</v>
+        <v>1.77</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -545,28 +545,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Review AM using Asset Change Tracker (5.5.13.1)</t>
+          <t>5.5.13 Real Property-Monthly Reviews-org</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Activity Step</t>
+          <t>Process</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>146</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F2" t="n">
-        <v>13</v>
+        <v>174</v>
       </c>
       <c r="G2" t="n">
-        <v>10.42</v>
+        <v>67.2</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -584,28 +584,28 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Complete /Accurate?</t>
+          <t>Review AM using Asset Change Tracker (5.5.13.1)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gateway</t>
+          <t>Activity Step</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
-        <v>146</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G3" t="n">
-        <v>1</v>
+        <v>9.75</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -623,7 +623,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Work with REO RPO to Correct (5.5.13.3)</t>
+          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -632,19 +632,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F4" t="n">
-        <v>165</v>
+        <v>5</v>
       </c>
       <c r="G4" t="n">
-        <v>117.12</v>
+        <v>4</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -662,67 +662,67 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
+          <t>Create/Post Journal Entries (5.5.13.4)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Activity Step</t>
+          <t>Stop</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>147</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F5" t="n">
         <v>6</v>
       </c>
       <c r="G5" t="n">
-        <v>3.84</v>
+        <v>5.4</v>
       </c>
       <c r="H5" t="n">
-        <v>1698</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>165</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>22.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Create/Post Journal Entries (5.5.13.4)</t>
+          <t>Work with REO RPO to Correct (5.5.13.3)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Stop</t>
+          <t>Activity Step</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
-        <v>144</v>
+        <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="F6" t="n">
-        <v>6</v>
+        <v>157</v>
       </c>
       <c r="G6" t="n">
-        <v>5.15</v>
+        <v>110.67</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -734,45 +734,6 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Stop</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>144</v>
-      </c>
-      <c r="D7" t="n">
-        <v>144</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wait time still not accurate.  Tokens counts in report do not match simulation_log
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.75</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.77</v>
+        <v>1.22</v>
       </c>
     </row>
   </sheetData>
@@ -557,16 +557,16 @@
         <v>10</v>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="G2" t="n">
-        <v>67.2</v>
+        <v>87.5</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -593,19 +593,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G3" t="n">
-        <v>9.75</v>
+        <v>9.4</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -623,7 +623,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
+          <t>Work with REO RPO to Correct (5.5.13.3)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -632,19 +632,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F4" t="n">
-        <v>5</v>
+        <v>150</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>139.5</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -662,28 +662,28 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Create/Post Journal Entries (5.5.13.4)</t>
+          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Stop</t>
+          <t>Activity Step</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F5" t="n">
         <v>6</v>
       </c>
       <c r="G5" t="n">
-        <v>5.4</v>
+        <v>3.5</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -701,28 +701,28 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Work with REO RPO to Correct (5.5.13.3)</t>
+          <t>Create/Post Journal Entries (5.5.13.4)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Activity Step</t>
+          <t>Stop</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
-        <v>80</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
-        <v>157</v>
+        <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>110.67</v>
+        <v>5.25</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added folder with test data to repo
</commit_message>
<xml_diff>
--- a/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
+++ b/5.5.13 Real Property-Monthly Reviews-org_results.xlsx
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.77</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.22</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,19 +554,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>87.5</v>
+        <v>0</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -578,162 +578,6 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Review AM using Asset Change Tracker (5.5.13.1)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" t="n">
-        <v>6</v>
-      </c>
-      <c r="F3" t="n">
-        <v>11</v>
-      </c>
-      <c r="G3" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Work with REO RPO to Correct (5.5.13.3)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>129</v>
-      </c>
-      <c r="F4" t="n">
-        <v>150</v>
-      </c>
-      <c r="G4" t="n">
-        <v>139.5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Note Accuracy in Asset Change Tracker (5.5.13.2)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Activity Step</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" t="n">
-        <v>6</v>
-      </c>
-      <c r="G5" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Create/Post Journal Entries (5.5.13.4)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Stop</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
-      <c r="G6" t="n">
-        <v>5.25</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>